<commit_message>
agregue metodo para escapar caracteres
</commit_message>
<xml_diff>
--- a/src/test/java/assets/Parametros.xlsx
+++ b/src/test/java/assets/Parametros.xlsx
@@ -1,54 +1,61 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20731"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{511D430B-322B-47A2-A2DF-9B3AE14CC65F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="60" windowWidth="12915" windowHeight="5190"/>
+    <workbookView xWindow="600" yWindow="60" windowWidth="12915" windowHeight="5190" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="179020"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+  <si>
+    <t>Product</t>
+  </si>
+  <si>
+    <t>Qty</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
   <si>
     <t>Fahrenheit 451 by Ray Bradbury</t>
   </si>
   <si>
-    <t>Product</t>
-  </si>
-  <si>
-    <t>Qty</t>
-  </si>
-  <si>
-    <t>Total</t>
-  </si>
-  <si>
     <t>$54.00</t>
   </si>
   <si>
     <t>Levi's 511 Jeans</t>
   </si>
   <si>
+    <t>$120.00</t>
+  </si>
+  <si>
     <t>Nokia Lumio 1020</t>
   </si>
   <si>
     <t>$349.00</t>
   </si>
   <si>
-    <t>$120.00</t>
+    <t>Nike SB Zoom Stefan Janoski "Medium Mint"</t>
+  </si>
+  <si>
+    <t>$30.00</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1">
     <font>
       <sz val="11"/>
@@ -116,12 +123,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -163,7 +173,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -195,9 +205,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -229,6 +257,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -404,32 +450,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="29.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B2" s="2">
         <v>2</v>
@@ -446,23 +492,34 @@
         <v>3</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4" s="2">
         <v>1</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="http://demo.nopcommerce.com/fahrenheit-451-by-ray-bradbury"/>
+    <hyperlink ref="A2" r:id="rId1" display="http://demo.nopcommerce.com/fahrenheit-451-by-ray-bradbury" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
@@ -470,24 +527,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" xr3:uid="{958C4451-9541-5A59-BF78-D2F731DF1C81}"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" xr3:uid="{842E5F09-E766-5B8D-85AF-A39847EA96FD}"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>